<commit_message>
Updated test plan and cases outline
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick\Documents\GitHub\RetroRobotsWoJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8640F183-AF89-4CFF-9AFB-0B1145D0087E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDC389B-F1B6-40F2-9774-0F6D3BB9CED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1207" windowWidth="18193" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
   <si>
     <t>Case</t>
   </si>
@@ -81,9 +81,6 @@
     <t>12 Category sectors placed randomly</t>
   </si>
   <si>
-    <t>Add POINTS to SCORE</t>
-  </si>
-  <si>
     <t>Store SCORE for first ROUND during second</t>
   </si>
   <si>
@@ -129,10 +126,16 @@
     <t>Game board</t>
   </si>
   <si>
-    <t>Player's scores</t>
-  </si>
-  <si>
-    <t>Buzzer</t>
+    <t>Player turn</t>
+  </si>
+  <si>
+    <t>Spin Button</t>
+  </si>
+  <si>
+    <t>Add POINTS to SCORE (correct answer)</t>
+  </si>
+  <si>
+    <t>Subtract POINTS to SCORE (incorrect answer)</t>
   </si>
 </sst>
 </file>
@@ -223,8 +226,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C9BB5DA-C786-439D-82F7-FC645716A5F1}" name="Table1" displayName="Table1" ref="A1:D80" totalsRowShown="0">
-  <autoFilter ref="A1:D80" xr:uid="{3C9BB5DA-C786-439D-82F7-FC645716A5F1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C9BB5DA-C786-439D-82F7-FC645716A5F1}" name="Table1" displayName="Table1" ref="A1:D83" totalsRowShown="0">
+  <autoFilter ref="A1:D83" xr:uid="{3C9BB5DA-C786-439D-82F7-FC645716A5F1}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{F18EA425-49B1-4D6D-B1FC-5E12DC7B75F1}" name="Requirement"/>
     <tableColumn id="6" xr3:uid="{721A8C16-EA15-4E92-B14B-B1A7299FD94B}" name="Case"/>
@@ -498,15 +501,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5859375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.29296875" customWidth="1"/>
     <col min="3" max="3" width="52.05859375" customWidth="1"/>
     <col min="4" max="4" width="30.703125" customWidth="1"/>
@@ -536,7 +539,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -544,17 +547,17 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -562,17 +565,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -580,17 +583,17 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -598,17 +601,17 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -616,17 +619,17 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -634,12 +637,12 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.5">
@@ -660,12 +663,12 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.5">
@@ -678,17 +681,17 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A28" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -696,17 +699,17 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A31" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -714,17 +717,17 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A34" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -732,17 +735,17 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A37" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -750,17 +753,17 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A40" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -768,12 +771,12 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.5">
@@ -786,7 +789,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A44" s="3" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -794,17 +797,17 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B46" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A47" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -812,29 +815,26 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+      <c r="A50" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A51" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="B51" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B52" t="s">
@@ -842,13 +842,16 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B53" t="s">
-        <v>29</v>
-      </c>
+      <c r="A53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A54" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -856,17 +859,17 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A57" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -874,17 +877,17 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B59" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A60" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -892,29 +895,26 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B61" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B62" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A63" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
+      <c r="A63" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A64" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
+      <c r="B64" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B65" t="s">
@@ -922,13 +922,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B66" t="s">
-        <v>29</v>
-      </c>
+      <c r="A66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A67" s="3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -936,29 +939,26 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A70" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
+      <c r="A70" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A71" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="B71" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B72" t="s">
@@ -966,13 +966,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B73" t="s">
-        <v>29</v>
-      </c>
+      <c r="A73" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A74" s="3" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -980,17 +983,17 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B75" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B76" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A77" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -998,12 +1001,30 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B78" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.5">
       <c r="B79" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A80" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B81" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B82" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated test cases and edited test plan
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick\Documents\GitHub\RetroRobotsWoJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE80B0E-1446-47D8-A5F0-3C12AD36671A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8D6E97-1925-41B0-B69E-5F045374A223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1507" yWindow="2007" windowWidth="24020" windowHeight="11526" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
   <si>
     <t>Case</t>
   </si>
@@ -214,6 +214,34 @@
   </si>
   <si>
     <t>Test Steps</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Round 2 is over</t>
+  </si>
+  <si>
+    <t>Expected winner for hard-coded dummy game is displayed as the game winner</t>
+  </si>
+  <si>
+    <t>1. Create a dummy game
+2. Set final score for all players
+3. Confirm show_winner() function returns correct player</t>
+  </si>
+  <si>
+    <t>Confirm what is displayed matches what is stored for player scores</t>
+  </si>
+  <si>
+    <t>1. Create a dummy game
+2. Set current scores
+3. Confirm correct scores are displayed</t>
+  </si>
+  <si>
+    <t>Hard-coded player scores should be the same as the scores displayed</t>
   </si>
 </sst>
 </file>
@@ -293,7 +321,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -341,16 +372,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C9BB5DA-C786-439D-82F7-FC645716A5F1}" name="Table1" displayName="Table1" ref="A1:G88" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:G88" xr:uid="{3C9BB5DA-C786-439D-82F7-FC645716A5F1}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F18EA425-49B1-4D6D-B1FC-5E12DC7B75F1}" name="Requirement" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{721A8C16-EA15-4E92-B14B-B1A7299FD94B}" name="Case" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{B7B50D22-EF10-4515-B9FA-B146B40A4F30}" name="Description" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{13BC7DF3-F0EC-49F1-87E3-3457F3E461B1}" name="Precondition" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{1833C2F2-93DD-425F-9EF6-3F709D80AF77}" name="Assumptions" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{7EF7C37A-97C2-42C1-AE08-888D02434045}" name="Test Steps" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{93B38700-C551-4A2D-AB12-628E35CC8936}" name="Notes" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C9BB5DA-C786-439D-82F7-FC645716A5F1}" name="Table1" displayName="Table1" ref="A1:H88" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H88" xr:uid="{3C9BB5DA-C786-439D-82F7-FC645716A5F1}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{F18EA425-49B1-4D6D-B1FC-5E12DC7B75F1}" name="Requirement" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{721A8C16-EA15-4E92-B14B-B1A7299FD94B}" name="Case" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{B7B50D22-EF10-4515-B9FA-B146B40A4F30}" name="Description" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{13BC7DF3-F0EC-49F1-87E3-3457F3E461B1}" name="Precondition" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{1833C2F2-93DD-425F-9EF6-3F709D80AF77}" name="Assumptions" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{7EF7C37A-97C2-42C1-AE08-888D02434045}" name="Test Steps" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{67F35970-CC48-4104-9E8F-8A6ADEBEFF37}" name="Expected Result" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{93B38700-C551-4A2D-AB12-628E35CC8936}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -619,25 +651,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="36.5859375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.3515625" style="1" customWidth="1"/>
-    <col min="3" max="6" width="52.05859375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.703125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.9375" style="1"/>
+    <col min="3" max="7" width="52.05859375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.9375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -657,10 +689,13 @@
         <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -670,8 +705,9 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -681,21 +717,49 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="43" x14ac:dyDescent="0.5">
       <c r="B4" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="C4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="43" x14ac:dyDescent="0.5">
       <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="D5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6" s="4" t="s">
         <v>28</v>
       </c>
@@ -705,18 +769,19 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B8" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A9" s="4" t="s">
         <v>31</v>
       </c>
@@ -726,8 +791,9 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B10" s="1" t="s">
         <v>44</v>
       </c>
@@ -735,7 +801,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
@@ -743,7 +809,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B12" s="1" t="s">
         <v>49</v>
       </c>
@@ -751,12 +817,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B13" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B14" s="1" t="s">
         <v>56</v>
       </c>
@@ -764,17 +830,17 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="43" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" ht="43" x14ac:dyDescent="0.5">
       <c r="B15" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B16" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
@@ -784,18 +850,19 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B18" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A20" s="4" t="s">
         <v>29</v>
       </c>
@@ -805,18 +872,19 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23" s="4" t="s">
         <v>32</v>
       </c>
@@ -826,8 +894,9 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B24" s="1" t="s">
         <v>53</v>
       </c>
@@ -835,7 +904,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B25" s="1" t="s">
         <v>52</v>
       </c>
@@ -843,7 +912,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -853,8 +922,9 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A27" s="4" t="s">
         <v>17</v>
       </c>
@@ -864,18 +934,19 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B28" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B29" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A30" s="4" t="s">
         <v>16</v>
       </c>
@@ -885,18 +956,19 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B32" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A33" s="4" t="s">
         <v>19</v>
       </c>
@@ -906,18 +978,19 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B34" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B35" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
@@ -927,18 +1000,19 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B37" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B38" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A39" s="4" t="s">
         <v>21</v>
       </c>
@@ -948,18 +1022,19 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B40" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B41" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A42" s="4" t="s">
         <v>22</v>
       </c>
@@ -969,18 +1044,19 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B44" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A45" s="4" t="s">
         <v>23</v>
       </c>
@@ -990,18 +1066,19 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B46" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B47" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A48" s="2" t="s">
         <v>5</v>
       </c>
@@ -1011,8 +1088,9 @@
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A49" s="4" t="s">
         <v>34</v>
       </c>
@@ -1022,18 +1100,19 @@
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B50" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B51" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A52" s="4" t="s">
         <v>33</v>
       </c>
@@ -1043,18 +1122,19 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B53" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B54" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A55" s="4" t="s">
         <v>18</v>
       </c>
@@ -1064,18 +1144,19 @@
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B56" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B57" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A58" s="2" t="s">
         <v>7</v>
       </c>
@@ -1085,8 +1166,9 @@
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A59" s="4" t="s">
         <v>11</v>
       </c>
@@ -1096,18 +1178,19 @@
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H59" s="4"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B60" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B61" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A62" s="4" t="s">
         <v>12</v>
       </c>
@@ -1117,18 +1200,19 @@
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B63" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B64" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A65" s="4" t="s">
         <v>13</v>
       </c>
@@ -1138,18 +1222,19 @@
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H65" s="4"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B66" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B67" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A68" s="4" t="s">
         <v>14</v>
       </c>
@@ -1159,18 +1244,19 @@
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H68" s="4"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B69" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B70" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A71" s="2" t="s">
         <v>8</v>
       </c>
@@ -1180,8 +1266,9 @@
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H71" s="3"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A72" s="4" t="s">
         <v>24</v>
       </c>
@@ -1191,18 +1278,19 @@
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H72" s="4"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B73" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B74" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A75" s="4" t="s">
         <v>10</v>
       </c>
@@ -1212,18 +1300,19 @@
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H75" s="4"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B76" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B77" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A78" s="2" t="s">
         <v>15</v>
       </c>
@@ -1233,8 +1322,9 @@
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H78" s="3"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A79" s="4" t="s">
         <v>9</v>
       </c>
@@ -1244,18 +1334,19 @@
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H79" s="4"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B80" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B81" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A82" s="4" t="s">
         <v>25</v>
       </c>
@@ -1265,18 +1356,19 @@
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H82" s="4"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B83" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B84" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A85" s="4" t="s">
         <v>26</v>
       </c>
@@ -1286,13 +1378,14 @@
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H85" s="4"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B86" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B87" s="1" t="s">
         <v>41</v>
       </c>

</xml_diff>